<commit_message>
[version 27] UNet + GHCU Method: REGRESSION location and HEATMAP visibility
</commit_message>
<xml_diff>
--- a/model_evaluate.xlsx
+++ b/model_evaluate.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
   <si>
     <t>model</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -99,6 +99,62 @@
   </si>
   <si>
     <t>epoch 100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>try-6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>epoch 130</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>try-7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>epoch 140</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>epoch 100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v22</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v21</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v23</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>epoch 100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v22-2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v22-3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>epoch 50</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v24</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>全猜visible</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -472,10 +528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H13"/>
+  <dimension ref="B1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="C2" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -488,10 +544,11 @@
     <col min="6" max="6" width="22.6640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="16.33203125" style="1" customWidth="1"/>
     <col min="8" max="8" width="18.6640625" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="1"/>
+    <col min="9" max="9" width="12.77734375" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8">
+    <row r="1" spans="2:9">
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
@@ -511,7 +568,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="2:8">
+    <row r="2" spans="2:9">
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
@@ -525,7 +582,7 @@
         <v>1.94823273867329E-2</v>
       </c>
     </row>
-    <row r="3" spans="2:8">
+    <row r="3" spans="2:9">
       <c r="E3" s="1" t="s">
         <v>7</v>
       </c>
@@ -536,7 +593,7 @@
         <v>0.55477197931358702</v>
       </c>
     </row>
-    <row r="4" spans="2:8">
+    <row r="4" spans="2:9">
       <c r="E4" s="1" t="s">
         <v>5</v>
       </c>
@@ -544,7 +601,7 @@
         <v>0.32554776348133302</v>
       </c>
     </row>
-    <row r="5" spans="2:8">
+    <row r="5" spans="2:9">
       <c r="E5" s="1" t="s">
         <v>1</v>
       </c>
@@ -552,7 +609,7 @@
         <v>1.3348059750989299E-2</v>
       </c>
     </row>
-    <row r="6" spans="2:8">
+    <row r="6" spans="2:9">
       <c r="E6" s="1" t="s">
         <v>8</v>
       </c>
@@ -563,7 +620,7 @@
         <v>0.82894530637830999</v>
       </c>
     </row>
-    <row r="7" spans="2:8">
+    <row r="7" spans="2:9">
       <c r="E7" s="1" t="s">
         <v>13</v>
       </c>
@@ -571,59 +628,159 @@
         <v>0.557055887457509</v>
       </c>
     </row>
-    <row r="9" spans="2:8">
+    <row r="8" spans="2:9">
+      <c r="E8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0.63815958611819401</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9">
       <c r="E9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0.316436661235521</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9">
+      <c r="E10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0.31132784627410198</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0.73397586585174701</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9">
+      <c r="E11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0.313779001121264</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9">
+      <c r="E12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0.34145764182721</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0.73405422347594396</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9">
+      <c r="E13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0.32692773974968298</v>
+      </c>
+      <c r="H13" s="1">
+        <v>0.51457451810061094</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9">
+      <c r="E15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G15" s="1">
         <v>0.45056718060942003</v>
       </c>
     </row>
-    <row r="10" spans="2:8">
-      <c r="E10" s="1" t="s">
+    <row r="16" spans="2:9">
+      <c r="E16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G16" s="1">
         <v>0.67767137182820103</v>
       </c>
     </row>
-    <row r="11" spans="2:8">
-      <c r="E11" s="1" t="s">
+    <row r="17" spans="5:7">
+      <c r="E17" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G17" s="1">
         <v>0.33276551248675501</v>
       </c>
     </row>
-    <row r="12" spans="2:8">
-      <c r="E12" s="1" t="s">
+    <row r="18" spans="5:7">
+      <c r="E18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G12" s="1">
+      <c r="G18" s="1">
         <v>0.73050270973277998</v>
       </c>
     </row>
-    <row r="13" spans="2:8">
-      <c r="E13" s="1" t="s">
+    <row r="19" spans="5:7">
+      <c r="E19" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F19" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G13" s="1">
+      <c r="G19" s="1">
         <v>0.44648081687005298</v>
+      </c>
+    </row>
+    <row r="20" spans="5:7">
+      <c r="E20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G20" s="1">
+        <v>0.32445426060138099</v>
+      </c>
+    </row>
+    <row r="21" spans="5:7">
+      <c r="E21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G21" s="1">
+        <v>0.330743415082632</v>
       </c>
     </row>
   </sheetData>

</xml_diff>